<commit_message>
Ajuste no cabeçalho da planilha
</commit_message>
<xml_diff>
--- a/src/assets/modelo/Layout importação facilitador.xlsx
+++ b/src/assets/modelo/Layout importação facilitador.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\projeto-facilitador\src\assets\modelo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27D894F1-54A6-4138-8BCB-4E06538DCDFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F66840D4-D544-4670-A7FA-58B0D60A6053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2FF833F1-11AE-40C4-AC4E-B6DE8CA6001B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2FF833F1-11AE-40C4-AC4E-B6DE8CA6001B}"/>
   </bookViews>
   <sheets>
     <sheet name="01_mch" sheetId="1" r:id="rId1"/>
@@ -31,13 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
-  <si>
-    <t>NOME FANTASIA</t>
-  </si>
-  <si>
-    <t>ENDEREÇO</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>BAIRRO</t>
   </si>
@@ -54,9 +48,6 @@
     <t>CNPJ</t>
   </si>
   <si>
-    <t>TITULOS</t>
-  </si>
-  <si>
     <t>PARCELA</t>
   </si>
   <si>
@@ -66,28 +57,46 @@
     <t xml:space="preserve">VALOR </t>
   </si>
   <si>
-    <t>SERASA</t>
-  </si>
-  <si>
-    <t>Tipo_titulo</t>
-  </si>
-  <si>
-    <t>plano</t>
-  </si>
-  <si>
-    <t>Numero</t>
-  </si>
-  <si>
-    <t>Celular whatsapp</t>
-  </si>
-  <si>
-    <t>Fone comercial</t>
-  </si>
-  <si>
-    <t>Fone residencial</t>
-  </si>
-  <si>
-    <t>Fone outros</t>
+    <t>NOME_FANTASIA</t>
+  </si>
+  <si>
+    <t>ENDERECO</t>
+  </si>
+  <si>
+    <t>NUMERO</t>
+  </si>
+  <si>
+    <t>TIPO_TITULO</t>
+  </si>
+  <si>
+    <t>PLANO</t>
+  </si>
+  <si>
+    <t>CONTRATO</t>
+  </si>
+  <si>
+    <t>DOCUMENTO</t>
+  </si>
+  <si>
+    <t>PRODUTO</t>
+  </si>
+  <si>
+    <t>CELULAR_WHATSAPP</t>
+  </si>
+  <si>
+    <t>FONE_COMERCIAL</t>
+  </si>
+  <si>
+    <t>FONE_RESIDENCIAL</t>
+  </si>
+  <si>
+    <t>FONE_OUTROS</t>
+  </si>
+  <si>
+    <t>EMAIL_1</t>
+  </si>
+  <si>
+    <t>EMAIL_2</t>
   </si>
 </sst>
 </file>
@@ -99,7 +108,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.00;[Red]#,##0.00"/>
     <numFmt numFmtId="165" formatCode="000000000000"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -230,6 +239,23 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -609,28 +635,29 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="33" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="16" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="18" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="33" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Ênfase1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -691,9 +718,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -731,7 +758,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -837,7 +864,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -979,7 +1006,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -987,95 +1014,100 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBC85475-CF46-42FE-9165-446BF5B875DB}">
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:V1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.77734375" customWidth="1"/>
-    <col min="4" max="4" width="14.21875" customWidth="1"/>
-    <col min="5" max="5" width="29" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="43.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.44140625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="5.6640625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="8.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.88671875" style="3" customWidth="1"/>
-    <col min="12" max="12" width="13.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="P1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>10</v>
-      </c>
       <c r="Q1" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="R1" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="S1" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="T1" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="U1" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="8" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>